<commit_message>
fleshing out the color mappings
</commit_message>
<xml_diff>
--- a/assets/Color Table.xlsx
+++ b/assets/Color Table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Default</t>
   </si>
@@ -27,15 +27,6 @@
     <t>Purple</t>
   </si>
   <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
     <t>#ca3c08</t>
   </si>
   <si>
@@ -99,38 +90,65 @@
     <t>5506a3</t>
   </si>
   <si>
-    <t>060aa3</t>
-  </si>
-  <si>
-    <t>2caa07</t>
-  </si>
-  <si>
-    <t>bd071b</t>
-  </si>
-  <si>
     <t>160d1f</t>
   </si>
   <si>
-    <t>0d0d1f</t>
-  </si>
-  <si>
-    <t>11200d</t>
-  </si>
-  <si>
-    <t>151b60</t>
-  </si>
-  <si>
-    <t>2e6416</t>
-  </si>
-  <si>
-    <t>6a1723</t>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>a:visited</t>
+  </si>
+  <si>
+    <t>button gradient</t>
+  </si>
+  <si>
+    <t>button border</t>
+  </si>
+  <si>
+    <t>button gradient (hover)</t>
+  </si>
+  <si>
+    <t>5d038a</t>
+  </si>
+  <si>
+    <t>7f22c3</t>
+  </si>
+  <si>
+    <t>490695</t>
+  </si>
+  <si>
+    <t>.entry-meta a, .entry-content a</t>
+  </si>
+  <si>
+    <t>a:active, a:hover, .entry-content a:hover</t>
+  </si>
+  <si>
+    <t>button gradient (hover), .paging-navigation .meta-nav</t>
+  </si>
+  <si>
+    <t>8029c7</t>
+  </si>
+  <si>
+    <t>741cba</t>
+  </si>
+  <si>
+    <t>6c21bf</t>
+  </si>
+  <si>
+    <t>5d0fb1</t>
+  </si>
+  <si>
+    <t>4d0898</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,6 +177,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,9 +210,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -526,173 +551,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="64.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="14" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="14" customHeight="1">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14" customHeight="1">
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>371560</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14" customHeight="1">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14" customHeight="1">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14" customHeight="1">
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14" customHeight="1">
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="14" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="14" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1">
-        <v>371560</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="14" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14" customHeight="1">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="14" customHeight="1">
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="14" customHeight="1">
-      <c r="A8" s="1" t="s">
+    <row r="17" spans="1:3" ht="14" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14" customHeight="1">
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14" customHeight="1">
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14" customHeight="1">
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14" customHeight="1">
+      <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="14" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="14" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="14" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="14" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="14" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="14" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="14" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="14" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="14" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="14" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="14" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="14" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="14" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A39">
-    <sortCondition ref="A2:A39"/>
+  <sortState ref="B2:B39">
+    <sortCondition ref="B2:B39"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>